<commit_message>
Adding accession numbers up to 90 ground truth (no detection points for those yet)
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_all.xlsx
+++ b/GHT/ground_truth_detection_pts_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\ESC499 - Thesis\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E906892-6CCA-4153-A277-A346FB0016D9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40835351-F8F6-4BCC-9050-F10013AE969D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>x</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>Need to Delete</t>
+  </si>
+  <si>
+    <t>60th Ground Truth Point</t>
+  </si>
+  <si>
+    <t>70th Ground Truth Point</t>
+  </si>
+  <si>
+    <t>80th Ground Truth Point</t>
+  </si>
+  <si>
+    <t>90th Ground Truth Point</t>
   </si>
 </sst>
 </file>
@@ -457,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1371,7 +1383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>8512802</v>
       </c>
@@ -1385,7 +1397,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>8540998</v>
       </c>
@@ -1399,7 +1411,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>8578004</v>
       </c>
@@ -1413,7 +1425,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>8609486</v>
       </c>
@@ -1425,6 +1437,188 @@
       </c>
       <c r="D68">
         <v>19</v>
+      </c>
+      <c r="E68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="2">
+        <v>8609024</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="2">
+        <v>8649140</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="2">
+        <v>8664266</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="2">
+        <v>8666303</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="2">
+        <v>8687072</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="2">
+        <v>8697536</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" s="2">
+        <v>8717421</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" s="2">
+        <v>8723551</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" s="2">
+        <v>8734298</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" s="2">
+        <v>8766117</v>
+      </c>
+      <c r="E78" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" s="2">
+        <v>8791550</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" s="2">
+        <v>8837927</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" s="2">
+        <v>8847103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" s="2">
+        <v>8864910</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" s="2">
+        <v>8915108</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" s="2">
+        <v>8920727</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" s="2">
+        <v>8931170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" s="2">
+        <v>8931305</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" s="2">
+        <v>8943923</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" s="2">
+        <v>8958140</v>
+      </c>
+      <c r="E88" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" s="2">
+        <v>8976584</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" s="2">
+        <v>8985647</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" s="2">
+        <v>9014200</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" s="2">
+        <v>9020776</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" s="2">
+        <v>9043600</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" s="2">
+        <v>9049401</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" s="2">
+        <v>9063971</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" s="2">
+        <v>9086188</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" s="2">
+        <v>9104767</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" s="2">
+        <v>9115352</v>
+      </c>
+      <c r="E98" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" s="2">
+        <v>9118382</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" s="2">
+        <v>9136320</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" s="2">
+        <v>9145963</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" s="2">
+        <v>9189512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added to 80 ground truth points
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_all.xlsx
+++ b/GHT/ground_truth_detection_pts_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\ESC499 - Thesis\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40835351-F8F6-4BCC-9050-F10013AE969D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE936BF8-547B-49B4-94D5-5E563B4F7341}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>x</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>90th Ground Truth Point</t>
+  </si>
+  <si>
+    <t>Not the type we are looking for</t>
+  </si>
+  <si>
+    <t>Not right</t>
   </si>
 </sst>
 </file>
@@ -471,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1444,53 +1450,143 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
-        <v>8609024</v>
+        <v>8649024</v>
+      </c>
+      <c r="B69">
+        <v>40</v>
+      </c>
+      <c r="C69">
+        <v>31</v>
+      </c>
+      <c r="D69">
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>8649140</v>
       </c>
+      <c r="B70">
+        <v>26</v>
+      </c>
+      <c r="C70">
+        <v>33</v>
+      </c>
+      <c r="D70">
+        <v>17</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>8664266</v>
       </c>
+      <c r="B71">
+        <v>29</v>
+      </c>
+      <c r="C71">
+        <v>53</v>
+      </c>
+      <c r="D71">
+        <v>19</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>8666303</v>
       </c>
+      <c r="B72">
+        <v>26</v>
+      </c>
+      <c r="C72">
+        <v>45</v>
+      </c>
+      <c r="D72">
+        <v>24</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>8687072</v>
       </c>
+      <c r="B73">
+        <v>23</v>
+      </c>
+      <c r="C73">
+        <v>45</v>
+      </c>
+      <c r="D73">
+        <v>23</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>8697536</v>
       </c>
+      <c r="B74">
+        <v>34</v>
+      </c>
+      <c r="C74">
+        <v>31</v>
+      </c>
+      <c r="D74">
+        <v>20</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>8717421</v>
       </c>
+      <c r="B75">
+        <v>32</v>
+      </c>
+      <c r="C75">
+        <v>54</v>
+      </c>
+      <c r="D75">
+        <v>20</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>8723551</v>
       </c>
+      <c r="B76">
+        <v>31</v>
+      </c>
+      <c r="C76">
+        <v>43</v>
+      </c>
+      <c r="D76">
+        <v>17</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>8734298</v>
       </c>
+      <c r="B77">
+        <v>31</v>
+      </c>
+      <c r="C77">
+        <v>55</v>
+      </c>
+      <c r="D77">
+        <v>21</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>8766117</v>
       </c>
+      <c r="B78">
+        <v>37</v>
+      </c>
+      <c r="C78">
+        <v>45</v>
+      </c>
+      <c r="D78">
+        <v>20</v>
+      </c>
       <c r="E78" t="s">
         <v>19</v>
       </c>
@@ -1499,63 +1595,159 @@
       <c r="A79" s="2">
         <v>8791550</v>
       </c>
+      <c r="B79">
+        <v>22</v>
+      </c>
+      <c r="C79">
+        <v>30</v>
+      </c>
+      <c r="D79">
+        <v>25</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>8837927</v>
       </c>
+      <c r="B80">
+        <v>32</v>
+      </c>
+      <c r="C80">
+        <v>46</v>
+      </c>
+      <c r="D80">
+        <v>24</v>
+      </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>8847103</v>
       </c>
+      <c r="B81">
+        <v>30</v>
+      </c>
+      <c r="C81">
+        <v>52</v>
+      </c>
+      <c r="D81">
+        <v>25</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>8864910</v>
       </c>
+      <c r="B82">
+        <v>27</v>
+      </c>
+      <c r="C82">
+        <v>51</v>
+      </c>
+      <c r="D82">
+        <v>30</v>
+      </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>8915108</v>
       </c>
+      <c r="E83" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>8920727</v>
       </c>
+      <c r="B84">
+        <v>21</v>
+      </c>
+      <c r="C84">
+        <v>47</v>
+      </c>
+      <c r="D84">
+        <v>24</v>
+      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>8931170</v>
       </c>
+      <c r="B85">
+        <v>31</v>
+      </c>
+      <c r="C85">
+        <v>48</v>
+      </c>
+      <c r="D85">
+        <v>25</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>8931305</v>
       </c>
+      <c r="B86">
+        <v>37</v>
+      </c>
+      <c r="C86">
+        <v>58</v>
+      </c>
+      <c r="D86">
+        <v>25</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>8943923</v>
       </c>
+      <c r="E87" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>8958140</v>
       </c>
-      <c r="E88" t="s">
-        <v>20</v>
+      <c r="B88">
+        <v>33</v>
+      </c>
+      <c r="C88">
+        <v>61</v>
+      </c>
+      <c r="D88">
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>8976584</v>
       </c>
+      <c r="B89">
+        <v>36</v>
+      </c>
+      <c r="C89">
+        <v>51</v>
+      </c>
+      <c r="D89">
+        <v>27</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>8985647</v>
+      </c>
+      <c r="B90">
+        <v>22</v>
+      </c>
+      <c r="C90">
+        <v>63</v>
+      </c>
+      <c r="D90">
+        <v>18</v>
+      </c>
+      <c r="E90" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added to 91 ground truth points
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_all.xlsx
+++ b/GHT/ground_truth_detection_pts_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\ESC499 - Thesis\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE936BF8-547B-49B4-94D5-5E563B4F7341}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4338EED-E20E-4307-AB6C-D04B9530226E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>x</t>
   </si>
@@ -87,12 +87,6 @@
     <t>Need to Delete</t>
   </si>
   <si>
-    <t>60th Ground Truth Point</t>
-  </si>
-  <si>
-    <t>70th Ground Truth Point</t>
-  </si>
-  <si>
     <t>80th Ground Truth Point</t>
   </si>
   <si>
@@ -103,6 +97,9 @@
   </si>
   <si>
     <t>Not right</t>
+  </si>
+  <si>
+    <t>Way too close to top</t>
   </si>
 </sst>
 </file>
@@ -477,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1389,7 +1386,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>8512802</v>
       </c>
@@ -1403,7 +1400,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>8540998</v>
       </c>
@@ -1417,7 +1414,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>8578004</v>
       </c>
@@ -1431,7 +1428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>8609486</v>
       </c>
@@ -1444,11 +1441,8 @@
       <c r="D68">
         <v>19</v>
       </c>
-      <c r="E68" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>8649024</v>
       </c>
@@ -1462,7 +1456,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>8649140</v>
       </c>
@@ -1476,7 +1470,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>8664266</v>
       </c>
@@ -1490,7 +1484,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>8666303</v>
       </c>
@@ -1504,7 +1498,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>8687072</v>
       </c>
@@ -1518,7 +1512,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>8697536</v>
       </c>
@@ -1532,7 +1526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>8717421</v>
       </c>
@@ -1546,7 +1540,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>8723551</v>
       </c>
@@ -1560,7 +1554,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>8734298</v>
       </c>
@@ -1574,7 +1568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>8766117</v>
       </c>
@@ -1587,11 +1581,8 @@
       <c r="D78">
         <v>20</v>
       </c>
-      <c r="E78" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>8791550</v>
       </c>
@@ -1605,7 +1596,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>8837927</v>
       </c>
@@ -1652,7 +1643,7 @@
         <v>8915108</v>
       </c>
       <c r="E83" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
@@ -1702,7 +1693,7 @@
         <v>8943923</v>
       </c>
       <c r="E87" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
@@ -1747,70 +1738,172 @@
         <v>18</v>
       </c>
       <c r="E90" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>9014200</v>
       </c>
+      <c r="B91">
+        <v>32</v>
+      </c>
+      <c r="C91">
+        <v>56</v>
+      </c>
+      <c r="D91">
+        <v>25</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>9020776</v>
       </c>
+      <c r="B92">
+        <v>41</v>
+      </c>
+      <c r="C92">
+        <v>50</v>
+      </c>
+      <c r="D92">
+        <v>27</v>
+      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>9043600</v>
       </c>
+      <c r="B93">
+        <v>40</v>
+      </c>
+      <c r="C93">
+        <v>47</v>
+      </c>
+      <c r="D93">
+        <v>24</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>9049401</v>
       </c>
+      <c r="B94">
+        <v>30</v>
+      </c>
+      <c r="C94">
+        <v>49</v>
+      </c>
+      <c r="D94">
+        <v>22</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>9063971</v>
       </c>
+      <c r="B95">
+        <v>26</v>
+      </c>
+      <c r="C95">
+        <v>46</v>
+      </c>
+      <c r="D95">
+        <v>20</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>9086188</v>
       </c>
+      <c r="B96">
+        <v>30</v>
+      </c>
+      <c r="C96">
+        <v>26</v>
+      </c>
+      <c r="D96">
+        <v>20</v>
+      </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>9104767</v>
       </c>
+      <c r="E97" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>9115352</v>
       </c>
-      <c r="E98" t="s">
-        <v>21</v>
+      <c r="B98">
+        <v>26</v>
+      </c>
+      <c r="C98">
+        <v>34</v>
+      </c>
+      <c r="D98">
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>9118382</v>
       </c>
+      <c r="B99">
+        <v>33</v>
+      </c>
+      <c r="C99">
+        <v>55</v>
+      </c>
+      <c r="D99">
+        <v>21</v>
+      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>9136320</v>
       </c>
+      <c r="B100">
+        <v>31</v>
+      </c>
+      <c r="C100">
+        <v>61</v>
+      </c>
+      <c r="D100">
+        <v>25</v>
+      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>9145963</v>
       </c>
+      <c r="B101">
+        <v>20</v>
+      </c>
+      <c r="C101">
+        <v>55</v>
+      </c>
+      <c r="D101">
+        <v>15</v>
+      </c>
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>9189512</v>
+      </c>
+      <c r="B102">
+        <v>37</v>
+      </c>
+      <c r="C102">
+        <v>57</v>
+      </c>
+      <c r="D102">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding up to a total of 101 valid ground truth points
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_all.xlsx
+++ b/GHT/ground_truth_detection_pts_all.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\ESC499 - Thesis\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4338EED-E20E-4307-AB6C-D04B9530226E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30403D11-BB51-4511-83CB-5DF62D1E4320}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -472,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,7 +485,7 @@
     <col min="5" max="5" width="54.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -494,7 +494,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -511,7 +511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>4491140</v>
       </c>
@@ -526,7 +526,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>4687879</v>
       </c>
@@ -540,433 +540,430 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
+        <v>4697342</v>
+      </c>
+      <c r="B5">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>4737315</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>66</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>4831559</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>4930402</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>59</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
         <v>5056218</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B9" s="2">
         <v>30</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C9" s="2">
         <v>49</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D9" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>5103832</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>5131203</v>
+      </c>
+      <c r="B11">
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>61</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
         <v>5199556</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B12" s="2">
         <v>36</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C12" s="2">
         <v>56</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D12" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
         <v>5235783</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B13" s="2">
         <v>35</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C13" s="2">
         <v>59</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D13" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>5334421</v>
+      </c>
+      <c r="B14">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
         <v>5372580</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B15" s="2">
         <v>25</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C15" s="2">
         <v>52</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D15" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>5411573</v>
+      </c>
+      <c r="B16">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>55</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
         <v>5433681</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B17" s="2">
         <v>36</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C17" s="2">
         <v>65</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D17" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
         <v>5506328</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B18" s="2">
         <v>28</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C18" s="2">
         <v>47</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D18" s="2">
         <v>14</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E18" t="s">
         <v>7</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
         <v>5523521</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B19" s="2">
         <v>28</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C19" s="2">
         <v>43</v>
-      </c>
-      <c r="D11" s="2">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
-        <v>5680178</v>
-      </c>
-      <c r="B12" s="2">
-        <v>31</v>
-      </c>
-      <c r="C12" s="2">
-        <v>59</v>
-      </c>
-      <c r="D12" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
-        <v>5739421</v>
-      </c>
-      <c r="B13" s="2">
-        <v>28</v>
-      </c>
-      <c r="C13" s="2">
-        <v>60</v>
-      </c>
-      <c r="D13" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
-        <v>5826444</v>
-      </c>
-      <c r="B14" s="2">
-        <v>34</v>
-      </c>
-      <c r="C14" s="2">
-        <v>57</v>
-      </c>
-      <c r="D14" s="2">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
-        <v>5835023</v>
-      </c>
-      <c r="B15" s="2">
-        <v>34</v>
-      </c>
-      <c r="C15" s="2">
-        <v>63</v>
-      </c>
-      <c r="D15" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>6022046</v>
-      </c>
-      <c r="B16" s="2">
-        <v>35</v>
-      </c>
-      <c r="C16" s="2">
-        <v>57</v>
-      </c>
-      <c r="D16" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>6029287</v>
-      </c>
-      <c r="B17" s="2">
-        <v>28</v>
-      </c>
-      <c r="C17" s="2">
-        <v>53</v>
-      </c>
-      <c r="D17" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
-        <v>6055185</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
-        <v>6067977</v>
-      </c>
-      <c r="B19" s="2">
-        <v>34</v>
-      </c>
-      <c r="C19" s="2">
-        <v>60</v>
       </c>
       <c r="D19" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>6095054</v>
-      </c>
-      <c r="B20" s="2">
-        <v>27</v>
-      </c>
-      <c r="C20" s="2">
+        <v>5544945</v>
+      </c>
+      <c r="B20">
+        <v>32</v>
+      </c>
+      <c r="C20">
         <v>43</v>
       </c>
-      <c r="D20" s="2">
-        <v>25</v>
-      </c>
-      <c r="E20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>6165341</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5680178</v>
+      </c>
+      <c r="B21" s="2">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2">
+        <v>59</v>
+      </c>
+      <c r="D21" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>6173842</v>
+        <v>5739421</v>
       </c>
       <c r="B22" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="2">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D22" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>6201211</v>
+        <v>5826444</v>
       </c>
       <c r="B23" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="D23" s="2">
         <v>17</v>
       </c>
       <c r="E23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>5835023</v>
+      </c>
+      <c r="B24" s="2">
+        <v>34</v>
+      </c>
+      <c r="C24" s="2">
+        <v>63</v>
+      </c>
+      <c r="D24" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>6022046</v>
+      </c>
+      <c r="B25" s="2">
+        <v>35</v>
+      </c>
+      <c r="C25" s="2">
+        <v>57</v>
+      </c>
+      <c r="D25" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>6029287</v>
+      </c>
+      <c r="B26" s="2">
+        <v>28</v>
+      </c>
+      <c r="C26" s="2">
+        <v>53</v>
+      </c>
+      <c r="D26" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>6055185</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>6067977</v>
+      </c>
+      <c r="B28" s="2">
+        <v>34</v>
+      </c>
+      <c r="C28" s="2">
+        <v>60</v>
+      </c>
+      <c r="D28" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>6095054</v>
+      </c>
+      <c r="B29" s="2">
+        <v>27</v>
+      </c>
+      <c r="C29" s="2">
+        <v>43</v>
+      </c>
+      <c r="D29" s="2">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>6165341</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>6173842</v>
+      </c>
+      <c r="B31" s="2">
+        <v>29</v>
+      </c>
+      <c r="C31" s="2">
+        <v>56</v>
+      </c>
+      <c r="D31" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>6201211</v>
+      </c>
+      <c r="B32" s="2">
+        <v>33</v>
+      </c>
+      <c r="C32" s="2">
+        <v>47</v>
+      </c>
+      <c r="D32" s="2">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
-        <v>6218246</v>
-      </c>
-      <c r="B24" s="2">
-        <v>29</v>
-      </c>
-      <c r="C24" s="2">
-        <v>61</v>
-      </c>
-      <c r="D24" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
-        <v>6268647</v>
-      </c>
-      <c r="B25" s="2">
-        <v>22</v>
-      </c>
-      <c r="C25" s="2">
-        <v>47</v>
-      </c>
-      <c r="D25" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
-        <v>6490491</v>
-      </c>
-      <c r="B26" s="2">
-        <v>30</v>
-      </c>
-      <c r="C26" s="2">
-        <v>54</v>
-      </c>
-      <c r="D26" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
-        <v>6729799</v>
-      </c>
-      <c r="B27" s="2">
-        <v>32</v>
-      </c>
-      <c r="C27" s="2">
-        <v>37</v>
-      </c>
-      <c r="D27" s="2">
-        <v>19</v>
-      </c>
-      <c r="E27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
-        <v>6828936</v>
-      </c>
-      <c r="B28" s="2">
-        <v>27</v>
-      </c>
-      <c r="C28" s="2">
-        <v>47</v>
-      </c>
-      <c r="D28" s="2">
-        <v>19</v>
-      </c>
-      <c r="E28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
-        <v>6868398</v>
-      </c>
-      <c r="B29" s="2">
-        <v>32</v>
-      </c>
-      <c r="C29" s="2">
-        <v>53</v>
-      </c>
-      <c r="D29" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
-        <v>6881614</v>
-      </c>
-      <c r="B30" s="2">
-        <v>29</v>
-      </c>
-      <c r="C30" s="2">
-        <v>55</v>
-      </c>
-      <c r="D30" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
-        <v>6993961</v>
-      </c>
-      <c r="B31" s="2">
-        <v>31</v>
-      </c>
-      <c r="C31" s="2">
-        <v>63</v>
-      </c>
-      <c r="D31" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2">
-        <v>7081341</v>
-      </c>
-      <c r="B32" s="2">
-        <v>29</v>
-      </c>
-      <c r="C32" s="2">
-        <v>51</v>
-      </c>
-      <c r="D32" s="2">
-        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
-        <v>7202530</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" t="s">
-        <v>14</v>
+        <v>6218246</v>
+      </c>
+      <c r="B33" s="2">
+        <v>29</v>
+      </c>
+      <c r="C33" s="2">
+        <v>61</v>
+      </c>
+      <c r="D33" s="2">
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
-        <v>7222303</v>
+        <v>6268647</v>
       </c>
       <c r="B34" s="2">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C34" s="2">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D34" s="2">
         <v>17</v>
@@ -974,737 +971,752 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
-        <v>7257259</v>
+        <v>6490491</v>
       </c>
       <c r="B35" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C35" s="2">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D35" s="2">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
-        <v>7299268</v>
+        <v>6729799</v>
       </c>
       <c r="B36" s="2">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C36" s="2">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D36" s="2">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
-        <v>7316415</v>
+        <v>6828936</v>
       </c>
       <c r="B37" s="2">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C37" s="2">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="D37" s="2">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
-        <v>7337296</v>
+        <v>6868398</v>
       </c>
       <c r="B38" s="2">
         <v>32</v>
       </c>
       <c r="C38" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D38" s="2">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
-        <v>7396455</v>
+        <v>6881614</v>
       </c>
       <c r="B39" s="2">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C39" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D39" s="2">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
-        <v>7444276</v>
+        <v>6993961</v>
       </c>
       <c r="B40" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C40" s="2">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D40" s="2">
-        <v>19</v>
-      </c>
-      <c r="E40" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
-        <v>7466141</v>
+        <v>7081341</v>
       </c>
       <c r="B41" s="2">
         <v>29</v>
       </c>
       <c r="C41" s="2">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D41" s="2">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
-        <v>7489680</v>
-      </c>
-      <c r="B42" s="2">
-        <v>33</v>
-      </c>
-      <c r="C42" s="2">
-        <v>53</v>
-      </c>
-      <c r="D42" s="2">
-        <v>19</v>
+        <v>7202530</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
-        <v>7496249</v>
+        <v>7222303</v>
       </c>
       <c r="B43" s="2">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C43" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D43" s="2">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
-        <v>7499820</v>
+        <v>7257259</v>
       </c>
       <c r="B44" s="2">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C44" s="2">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D44" s="2">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
-        <v>7629097</v>
+        <v>7299268</v>
       </c>
       <c r="B45" s="2">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C45" s="2">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D45" s="2">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
-        <v>7796800</v>
+        <v>7316415</v>
       </c>
       <c r="B46" s="2">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C46" s="2">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D46" s="2">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
-        <v>7800424</v>
+        <v>7337296</v>
       </c>
       <c r="B47" s="2">
-        <v>19</v>
-      </c>
-      <c r="C47">
-        <v>50</v>
+        <v>32</v>
+      </c>
+      <c r="C47" s="2">
+        <v>51</v>
       </c>
       <c r="D47" s="2">
-        <v>21</v>
-      </c>
-      <c r="E47" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
-        <v>7887075</v>
+        <v>7396455</v>
       </c>
       <c r="B48" s="2">
-        <v>36</v>
-      </c>
-      <c r="C48">
-        <v>60</v>
+        <v>48</v>
+      </c>
+      <c r="C48" s="2">
+        <v>54</v>
       </c>
       <c r="D48" s="2">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
-        <v>7958084</v>
+        <v>7444276</v>
       </c>
       <c r="B49" s="2">
-        <v>32</v>
-      </c>
-      <c r="C49">
-        <v>52</v>
+        <v>26</v>
+      </c>
+      <c r="C49" s="2">
+        <v>50</v>
       </c>
       <c r="D49" s="2">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="E49" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
-        <v>7962433</v>
+        <v>7466141</v>
       </c>
       <c r="B50" s="2">
         <v>29</v>
       </c>
-      <c r="C50">
-        <v>63</v>
+      <c r="C50" s="2">
+        <v>62</v>
       </c>
       <c r="D50" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
-        <v>7977808</v>
-      </c>
-      <c r="E51" t="s">
-        <v>17</v>
+        <v>7489680</v>
+      </c>
+      <c r="B51" s="2">
+        <v>33</v>
+      </c>
+      <c r="C51" s="2">
+        <v>53</v>
+      </c>
+      <c r="D51" s="2">
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
-        <v>8108990</v>
-      </c>
-      <c r="B52">
+        <v>7496249</v>
+      </c>
+      <c r="B52" s="2">
         <v>23</v>
       </c>
-      <c r="C52">
-        <v>46</v>
-      </c>
-      <c r="D52">
+      <c r="C52" s="2">
+        <v>50</v>
+      </c>
+      <c r="D52" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
-        <v>8207522</v>
-      </c>
-      <c r="E53" t="s">
-        <v>17</v>
+        <v>7499820</v>
+      </c>
+      <c r="B53" s="2">
+        <v>31</v>
+      </c>
+      <c r="C53" s="2">
+        <v>50</v>
+      </c>
+      <c r="D53" s="2">
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
-        <v>8214092</v>
-      </c>
-      <c r="B54">
-        <v>30</v>
-      </c>
-      <c r="C54">
-        <v>55</v>
-      </c>
-      <c r="D54">
-        <v>19</v>
+        <v>7629097</v>
+      </c>
+      <c r="B54" s="2">
+        <v>33</v>
+      </c>
+      <c r="C54" s="2">
+        <v>42</v>
+      </c>
+      <c r="D54" s="2">
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
-        <v>8280387</v>
-      </c>
-      <c r="B55">
-        <v>31</v>
-      </c>
-      <c r="C55">
-        <v>48</v>
-      </c>
-      <c r="D55">
-        <v>21</v>
+        <v>7796800</v>
+      </c>
+      <c r="B55" s="2">
+        <v>29</v>
+      </c>
+      <c r="C55" s="2">
+        <v>52</v>
+      </c>
+      <c r="D55" s="2">
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
-        <v>8285119</v>
-      </c>
-      <c r="B56">
-        <v>28</v>
+        <v>7800424</v>
+      </c>
+      <c r="B56" s="2">
+        <v>19</v>
       </c>
       <c r="C56">
-        <v>49</v>
-      </c>
-      <c r="D56">
-        <v>18</v>
+        <v>50</v>
+      </c>
+      <c r="D56" s="2">
+        <v>21</v>
+      </c>
+      <c r="E56" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
-        <v>8399974</v>
-      </c>
-      <c r="B57">
+        <v>7887075</v>
+      </c>
+      <c r="B57" s="2">
         <v>36</v>
       </c>
       <c r="C57">
-        <v>58</v>
-      </c>
-      <c r="D57">
-        <v>18</v>
+        <v>60</v>
+      </c>
+      <c r="D57" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
-        <v>8412228</v>
-      </c>
-      <c r="B58">
-        <v>26</v>
+        <v>7958084</v>
+      </c>
+      <c r="B58" s="2">
+        <v>32</v>
       </c>
       <c r="C58">
-        <v>50</v>
-      </c>
-      <c r="D58">
-        <v>22</v>
+        <v>52</v>
+      </c>
+      <c r="D58" s="2">
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
-        <v>8417665</v>
-      </c>
-      <c r="B59">
-        <v>33</v>
+        <v>7962433</v>
+      </c>
+      <c r="B59" s="2">
+        <v>29</v>
       </c>
       <c r="C59">
-        <v>59</v>
-      </c>
-      <c r="D59">
-        <v>21</v>
+        <v>63</v>
+      </c>
+      <c r="D59" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
-        <v>8419199</v>
-      </c>
-      <c r="B60">
-        <v>32</v>
-      </c>
-      <c r="C60">
-        <v>31</v>
-      </c>
-      <c r="D60">
-        <v>20</v>
+        <v>7977808</v>
+      </c>
+      <c r="E60" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
-        <v>8437096</v>
+        <v>8108990</v>
       </c>
       <c r="B61">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C61">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="D61">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
-        <v>8441021</v>
-      </c>
-      <c r="B62">
-        <v>32</v>
-      </c>
-      <c r="C62">
-        <v>56</v>
-      </c>
-      <c r="D62">
+        <v>8207522</v>
+      </c>
+      <c r="E62" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
-        <v>8476267</v>
+        <v>8214092</v>
       </c>
       <c r="B63">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C63">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D63">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
-        <v>8509076</v>
+        <v>8280387</v>
       </c>
       <c r="B64">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C64">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D64">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
-        <v>8512802</v>
+        <v>8285119</v>
       </c>
       <c r="B65">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C65">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D65">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
-        <v>8540998</v>
+        <v>8399974</v>
       </c>
       <c r="B66">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C66">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D66">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
-        <v>8578004</v>
+        <v>8412228</v>
       </c>
       <c r="B67">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C67">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D67">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
-        <v>8609486</v>
+        <v>8417665</v>
       </c>
       <c r="B68">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C68">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D68">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
-        <v>8649024</v>
+        <v>8419199</v>
       </c>
       <c r="B69">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C69">
         <v>31</v>
       </c>
       <c r="D69">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
-        <v>8649140</v>
+        <v>8437096</v>
       </c>
       <c r="B70">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C70">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D70">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
-        <v>8664266</v>
+        <v>8441021</v>
       </c>
       <c r="B71">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C71">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D71">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
-        <v>8666303</v>
+        <v>8476267</v>
       </c>
       <c r="B72">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C72">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D72">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
-        <v>8687072</v>
+        <v>8509076</v>
       </c>
       <c r="B73">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C73">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D73">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
-        <v>8697536</v>
+        <v>8512802</v>
       </c>
       <c r="B74">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C74">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D74">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
-        <v>8717421</v>
+        <v>8540998</v>
       </c>
       <c r="B75">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C75">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D75">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
-        <v>8723551</v>
+        <v>8578004</v>
       </c>
       <c r="B76">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C76">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D76">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
-        <v>8734298</v>
+        <v>8609486</v>
       </c>
       <c r="B77">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C77">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D77">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
-        <v>8766117</v>
+        <v>8649024</v>
       </c>
       <c r="B78">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C78">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D78">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
-        <v>8791550</v>
+        <v>8649140</v>
       </c>
       <c r="B79">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C79">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D79">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
-        <v>8837927</v>
+        <v>8664266</v>
       </c>
       <c r="B80">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C80">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D80">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
-        <v>8847103</v>
+        <v>8666303</v>
       </c>
       <c r="B81">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C81">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D81">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
-        <v>8864910</v>
+        <v>8687072</v>
       </c>
       <c r="B82">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C82">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D82">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
-        <v>8915108</v>
-      </c>
-      <c r="E83" t="s">
+        <v>8697536</v>
+      </c>
+      <c r="B83">
+        <v>34</v>
+      </c>
+      <c r="C83">
+        <v>31</v>
+      </c>
+      <c r="D83">
         <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
-        <v>8920727</v>
+        <v>8717421</v>
       </c>
       <c r="B84">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C84">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D84">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
-        <v>8931170</v>
+        <v>8723551</v>
       </c>
       <c r="B85">
         <v>31</v>
       </c>
       <c r="C85">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D85">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
-        <v>8931305</v>
+        <v>8734298</v>
       </c>
       <c r="B86">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C86">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D86">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
-        <v>8943923</v>
-      </c>
-      <c r="E87" t="s">
-        <v>21</v>
+        <v>8766117</v>
+      </c>
+      <c r="B87">
+        <v>37</v>
+      </c>
+      <c r="C87">
+        <v>45</v>
+      </c>
+      <c r="D87">
+        <v>20</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
-        <v>8958140</v>
+        <v>8791550</v>
       </c>
       <c r="B88">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C88">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="D88">
         <v>25</v>
@@ -1712,69 +1724,60 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
-        <v>8976584</v>
+        <v>8837927</v>
       </c>
       <c r="B89">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C89">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D89">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
-        <v>8985647</v>
+        <v>8847103</v>
       </c>
       <c r="B90">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C90">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D90">
-        <v>18</v>
-      </c>
-      <c r="E90" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
-        <v>9014200</v>
+        <v>8864910</v>
       </c>
       <c r="B91">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C91">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D91">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
-        <v>9020776</v>
-      </c>
-      <c r="B92">
-        <v>41</v>
-      </c>
-      <c r="C92">
-        <v>50</v>
-      </c>
-      <c r="D92">
-        <v>27</v>
+        <v>8915108</v>
+      </c>
+      <c r="E92" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
-        <v>9043600</v>
+        <v>8920727</v>
       </c>
       <c r="B93">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C93">
         <v>47</v>
@@ -1785,91 +1788,94 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
-        <v>9049401</v>
+        <v>8931170</v>
       </c>
       <c r="B94">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C94">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D94">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
-        <v>9063971</v>
+        <v>8931305</v>
       </c>
       <c r="B95">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C95">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D95">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
-        <v>9086188</v>
-      </c>
-      <c r="B96">
-        <v>30</v>
-      </c>
-      <c r="C96">
-        <v>26</v>
-      </c>
-      <c r="D96">
-        <v>20</v>
+        <v>8943923</v>
+      </c>
+      <c r="E96" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
-        <v>9104767</v>
-      </c>
-      <c r="E97" t="s">
-        <v>22</v>
+        <v>8958140</v>
+      </c>
+      <c r="B97">
+        <v>33</v>
+      </c>
+      <c r="C97">
+        <v>61</v>
+      </c>
+      <c r="D97">
+        <v>25</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
-        <v>9115352</v>
+        <v>8976584</v>
       </c>
       <c r="B98">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C98">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D98">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
-        <v>9118382</v>
+        <v>8985647</v>
       </c>
       <c r="B99">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C99">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D99">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="E99" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
-        <v>9136320</v>
+        <v>9014200</v>
       </c>
       <c r="B100">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C100">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D100">
         <v>25</v>
@@ -1877,38 +1883,158 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
-        <v>9145963</v>
+        <v>9020776</v>
       </c>
       <c r="B101">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C101">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D101">
-        <v>15</v>
-      </c>
-      <c r="E101" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
+        <v>9043600</v>
+      </c>
+      <c r="B102">
+        <v>40</v>
+      </c>
+      <c r="C102">
+        <v>47</v>
+      </c>
+      <c r="D102">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" s="2">
+        <v>9049401</v>
+      </c>
+      <c r="B103">
+        <v>30</v>
+      </c>
+      <c r="C103">
+        <v>49</v>
+      </c>
+      <c r="D103">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" s="2">
+        <v>9063971</v>
+      </c>
+      <c r="B104">
+        <v>26</v>
+      </c>
+      <c r="C104">
+        <v>46</v>
+      </c>
+      <c r="D104">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" s="2">
+        <v>9086188</v>
+      </c>
+      <c r="B105">
+        <v>30</v>
+      </c>
+      <c r="C105">
+        <v>26</v>
+      </c>
+      <c r="D105">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" s="2">
+        <v>9104767</v>
+      </c>
+      <c r="E106" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" s="2">
+        <v>9115352</v>
+      </c>
+      <c r="B107">
+        <v>26</v>
+      </c>
+      <c r="C107">
+        <v>34</v>
+      </c>
+      <c r="D107">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" s="2">
+        <v>9118382</v>
+      </c>
+      <c r="B108">
+        <v>33</v>
+      </c>
+      <c r="C108">
+        <v>55</v>
+      </c>
+      <c r="D108">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" s="2">
+        <v>9136320</v>
+      </c>
+      <c r="B109">
+        <v>31</v>
+      </c>
+      <c r="C109">
+        <v>61</v>
+      </c>
+      <c r="D109">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" s="2">
+        <v>9145963</v>
+      </c>
+      <c r="B110">
+        <v>20</v>
+      </c>
+      <c r="C110">
+        <v>55</v>
+      </c>
+      <c r="D110">
+        <v>15</v>
+      </c>
+      <c r="E110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" s="2">
         <v>9189512</v>
       </c>
-      <c r="B102">
+      <c r="B111">
         <v>37</v>
       </c>
-      <c r="C102">
+      <c r="C111">
         <v>57</v>
       </c>
-      <c r="D102">
+      <c r="D111">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E13">
-    <sortCondition ref="A4"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F111">
+    <sortCondition ref="A75"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
Modifying first half of ground truth reference points
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_all.xlsx
+++ b/GHT/ground_truth_detection_pts_all.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\ESC499 - Thesis\Undergraduate_Thesis_Scripts\GHT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\ESC499\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30403D11-BB51-4511-83CB-5DF62D1E4320}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3024AB1-9BC3-4110-8FDF-3559173F7FDA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12098" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Boundaries" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>x</t>
   </si>
@@ -100,6 +99,12 @@
   </si>
   <si>
     <t>Way too close to top</t>
+  </si>
+  <si>
+    <t>Quite off</t>
+  </si>
+  <si>
+    <t>Went up to here in updates</t>
   </si>
 </sst>
 </file>
@@ -474,18 +479,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="54.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.59765625" customWidth="1"/>
+    <col min="2" max="4" width="6.59765625" customWidth="1"/>
+    <col min="5" max="5" width="54.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -494,7 +499,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -511,22 +516,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>4491140</v>
       </c>
       <c r="B3" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D3" s="2">
         <v>18</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>4687879</v>
       </c>
@@ -534,13 +539,13 @@
         <v>32</v>
       </c>
       <c r="C4" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4697342</v>
       </c>
@@ -548,13 +553,13 @@
         <v>29</v>
       </c>
       <c r="C5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>4737315</v>
       </c>
@@ -568,7 +573,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>4831559</v>
       </c>
@@ -582,7 +587,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>4930402</v>
       </c>
@@ -596,12 +601,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>5056218</v>
       </c>
       <c r="B9" s="2">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2">
         <v>49</v>
@@ -610,7 +615,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>5103832</v>
       </c>
@@ -624,7 +629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>5131203</v>
       </c>
@@ -638,12 +643,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>5199556</v>
       </c>
       <c r="B12" s="2">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2">
         <v>56</v>
@@ -652,12 +657,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>5235783</v>
       </c>
       <c r="B13" s="2">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2">
         <v>59</v>
@@ -666,7 +671,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>5334421</v>
       </c>
@@ -674,27 +679,27 @@
         <v>19</v>
       </c>
       <c r="C14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>5372580</v>
       </c>
       <c r="B15" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D15" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>5411573</v>
       </c>
@@ -708,29 +713,32 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>5433681</v>
       </c>
       <c r="B17" s="2">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D17" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>5506328</v>
       </c>
       <c r="B18" s="2">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C18" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2">
         <v>14</v>
@@ -742,15 +750,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>5523521</v>
       </c>
       <c r="B19" s="2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D19" s="2">
         <v>18</v>
@@ -759,7 +767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>5544945</v>
       </c>
@@ -773,7 +781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>5680178</v>
       </c>
@@ -781,13 +789,13 @@
         <v>31</v>
       </c>
       <c r="C21" s="2">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D21" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>5739421</v>
       </c>
@@ -801,15 +809,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>5826444</v>
       </c>
       <c r="B23" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D23" s="2">
         <v>17</v>
@@ -818,49 +826,49 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>5835023</v>
       </c>
       <c r="B24" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D24" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>6022046</v>
       </c>
       <c r="B25" s="2">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C25" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D25" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>6029287</v>
       </c>
       <c r="B26" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D26" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>6055185</v>
       </c>
@@ -871,12 +879,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>6067977</v>
       </c>
       <c r="B28" s="2">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28" s="2">
         <v>60</v>
@@ -885,15 +893,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>6095054</v>
       </c>
       <c r="B29" s="2">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C29" s="2">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D29" s="2">
         <v>25</v>
@@ -902,7 +910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>6165341</v>
       </c>
@@ -910,7 +918,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>6173842</v>
       </c>
@@ -924,7 +932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>6201211</v>
       </c>
@@ -941,21 +949,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>6218246</v>
       </c>
       <c r="B33" s="2">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C33" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D33" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>6268647</v>
       </c>
@@ -963,35 +971,35 @@
         <v>22</v>
       </c>
       <c r="C34" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D34" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>6490491</v>
       </c>
       <c r="B35" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C35" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D35" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>6729799</v>
       </c>
       <c r="B36" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C36" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D36" s="2">
         <v>19</v>
@@ -1000,15 +1008,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>6828936</v>
       </c>
       <c r="B37" s="2">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C37" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" s="2">
         <v>19</v>
@@ -1017,12 +1025,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>6868398</v>
       </c>
       <c r="B38" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="2">
         <v>53</v>
@@ -1031,49 +1039,49 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>6881614</v>
       </c>
       <c r="B39" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C39" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D39" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>6993961</v>
       </c>
       <c r="B40" s="2">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C40" s="2">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D40" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>7081341</v>
       </c>
       <c r="B41" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C41" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D41" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>7202530</v>
       </c>
@@ -1084,21 +1092,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>7222303</v>
       </c>
       <c r="B43" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C43" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D43" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>7257259</v>
       </c>
@@ -1106,77 +1114,77 @@
         <v>29</v>
       </c>
       <c r="C44" s="2">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D44" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>7299268</v>
       </c>
       <c r="B45" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C45" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D45" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>7316415</v>
       </c>
       <c r="B46" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C46" s="2">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D46" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>7337296</v>
       </c>
       <c r="B47" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C47" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D47" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>7396455</v>
       </c>
       <c r="B48" s="2">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C48" s="2">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D48" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>7444276</v>
       </c>
       <c r="B49" s="2">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C49" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D49" s="2">
         <v>19</v>
@@ -1185,49 +1193,49 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>7466141</v>
       </c>
       <c r="B50" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C50" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D50" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>7489680</v>
       </c>
       <c r="B51" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C51" s="2">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D51" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>7496249</v>
       </c>
       <c r="B52" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C52" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D52" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>7499820</v>
       </c>
@@ -1241,12 +1249,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>7629097</v>
       </c>
       <c r="B54" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C54" s="2">
         <v>42</v>
@@ -1255,29 +1263,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>7796800</v>
       </c>
       <c r="B55" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C55" s="2">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D55" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>7800424</v>
       </c>
       <c r="B56" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C56">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D56" s="2">
         <v>21</v>
@@ -1286,7 +1294,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>7887075</v>
       </c>
@@ -1300,7 +1308,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>7958084</v>
       </c>
@@ -1308,13 +1316,13 @@
         <v>32</v>
       </c>
       <c r="C58">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D58" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>7962433</v>
       </c>
@@ -1328,7 +1336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>7977808</v>
       </c>
@@ -1336,21 +1344,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>8108990</v>
       </c>
       <c r="B61">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C61">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D61">
         <v>21</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E61" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
         <v>8207522</v>
       </c>
@@ -1358,7 +1369,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
         <v>8214092</v>
       </c>
@@ -1372,7 +1383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
         <v>8280387</v>
       </c>
@@ -1386,7 +1397,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>8285119</v>
       </c>
@@ -1400,7 +1411,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>8399974</v>
       </c>
@@ -1414,7 +1425,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>8412228</v>
       </c>
@@ -1428,7 +1439,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
         <v>8417665</v>
       </c>
@@ -1442,7 +1453,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
         <v>8419199</v>
       </c>
@@ -1456,7 +1467,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
         <v>8437096</v>
       </c>
@@ -1470,7 +1481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>8441021</v>
       </c>
@@ -1484,7 +1495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>8476267</v>
       </c>
@@ -1498,7 +1509,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>8509076</v>
       </c>
@@ -1512,7 +1523,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
         <v>8512802</v>
       </c>
@@ -1526,7 +1537,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
         <v>8540998</v>
       </c>
@@ -1540,7 +1551,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
         <v>8578004</v>
       </c>
@@ -1554,7 +1565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>8609486</v>
       </c>
@@ -1568,7 +1579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>8649024</v>
       </c>
@@ -1582,7 +1593,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>8649140</v>
       </c>
@@ -1596,7 +1607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
         <v>8664266</v>
       </c>
@@ -1610,7 +1621,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
         <v>8666303</v>
       </c>
@@ -1624,7 +1635,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
         <v>8687072</v>
       </c>
@@ -1638,7 +1649,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>8697536</v>
       </c>
@@ -1652,7 +1663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>8717421</v>
       </c>
@@ -1666,7 +1677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A85" s="2">
         <v>8723551</v>
       </c>
@@ -1680,7 +1691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A86" s="2">
         <v>8734298</v>
       </c>
@@ -1694,7 +1705,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A87" s="2">
         <v>8766117</v>
       </c>
@@ -1708,7 +1719,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A88" s="2">
         <v>8791550</v>
       </c>
@@ -1722,7 +1733,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>8837927</v>
       </c>
@@ -1736,7 +1747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A90" s="2">
         <v>8847103</v>
       </c>
@@ -1750,7 +1761,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A91" s="2">
         <v>8864910</v>
       </c>
@@ -1764,7 +1775,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>8915108</v>
       </c>
@@ -1772,7 +1783,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A93" s="2">
         <v>8920727</v>
       </c>
@@ -1786,7 +1797,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A94" s="2">
         <v>8931170</v>
       </c>
@@ -1800,7 +1811,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A95" s="2">
         <v>8931305</v>
       </c>
@@ -1814,7 +1825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A96" s="2">
         <v>8943923</v>
       </c>
@@ -1822,7 +1833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" s="2">
         <v>8958140</v>
       </c>
@@ -1836,7 +1847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>8976584</v>
       </c>
@@ -1850,7 +1861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A99" s="2">
         <v>8985647</v>
       </c>
@@ -1867,7 +1878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A100" s="2">
         <v>9014200</v>
       </c>
@@ -1881,7 +1892,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A101" s="2">
         <v>9020776</v>
       </c>
@@ -1895,7 +1906,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A102" s="2">
         <v>9043600</v>
       </c>
@@ -1909,7 +1920,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A103" s="2">
         <v>9049401</v>
       </c>
@@ -1923,7 +1934,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A104" s="2">
         <v>9063971</v>
       </c>
@@ -1937,7 +1948,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A105" s="2">
         <v>9086188</v>
       </c>
@@ -1951,7 +1962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A106" s="2">
         <v>9104767</v>
       </c>
@@ -1959,7 +1970,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A107" s="2">
         <v>9115352</v>
       </c>
@@ -1973,7 +1984,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A108" s="2">
         <v>9118382</v>
       </c>
@@ -1987,7 +1998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A109" s="2">
         <v>9136320</v>
       </c>
@@ -2001,7 +2012,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A110" s="2">
         <v>9145963</v>
       </c>
@@ -2018,7 +2029,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A111" s="2">
         <v>9189512</v>
       </c>
@@ -2033,7 +2044,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F111">
+  <sortState ref="A3:F111">
     <sortCondition ref="A75"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Modifying second half of ground truth reference points
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_all.xlsx
+++ b/GHT/ground_truth_detection_pts_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\ESC499\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3024AB1-9BC3-4110-8FDF-3559173F7FDA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096DA82E-033B-493D-9247-738A13A51189}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12098" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>x</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Quite off</t>
-  </si>
-  <si>
-    <t>Went up to here in updates</t>
   </si>
 </sst>
 </file>
@@ -479,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1357,9 +1354,6 @@
       <c r="D61">
         <v>21</v>
       </c>
-      <c r="E61" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
@@ -1374,10 +1368,10 @@
         <v>8214092</v>
       </c>
       <c r="B63">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C63">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D63">
         <v>19</v>
@@ -1388,10 +1382,10 @@
         <v>8280387</v>
       </c>
       <c r="B64">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C64">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D64">
         <v>21</v>
@@ -1405,7 +1399,7 @@
         <v>28</v>
       </c>
       <c r="C65">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D65">
         <v>18</v>
@@ -1461,7 +1455,7 @@
         <v>32</v>
       </c>
       <c r="C69">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D69">
         <v>20</v>
@@ -1486,7 +1480,7 @@
         <v>8441021</v>
       </c>
       <c r="B71">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C71">
         <v>56</v>
@@ -1517,7 +1511,7 @@
         <v>39</v>
       </c>
       <c r="C73">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D73">
         <v>24</v>
@@ -1531,7 +1525,7 @@
         <v>30</v>
       </c>
       <c r="C74">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D74">
         <v>21</v>
@@ -1542,10 +1536,10 @@
         <v>8540998</v>
       </c>
       <c r="B75">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C75">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D75">
         <v>25</v>
@@ -1559,7 +1553,7 @@
         <v>33</v>
       </c>
       <c r="C76">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D76">
         <v>20</v>
@@ -1573,7 +1567,7 @@
         <v>36</v>
       </c>
       <c r="C77">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D77">
         <v>19</v>
@@ -1587,7 +1581,7 @@
         <v>40</v>
       </c>
       <c r="C78">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D78">
         <v>21</v>
@@ -1615,7 +1609,7 @@
         <v>29</v>
       </c>
       <c r="C80">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D80">
         <v>19</v>
@@ -1643,7 +1637,7 @@
         <v>23</v>
       </c>
       <c r="C82">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D82">
         <v>23</v>
@@ -1654,10 +1648,10 @@
         <v>8697536</v>
       </c>
       <c r="B83">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C83">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D83">
         <v>20</v>
@@ -1668,10 +1662,10 @@
         <v>8717421</v>
       </c>
       <c r="B84">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C84">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D84">
         <v>20</v>
@@ -1710,10 +1704,10 @@
         <v>8766117</v>
       </c>
       <c r="B87">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C87">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D87">
         <v>20</v>
@@ -1727,7 +1721,7 @@
         <v>22</v>
       </c>
       <c r="C88">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D88">
         <v>25</v>
@@ -1741,7 +1735,7 @@
         <v>32</v>
       </c>
       <c r="C89">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D89">
         <v>24</v>
@@ -1755,7 +1749,7 @@
         <v>30</v>
       </c>
       <c r="C90">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D90">
         <v>25</v>
@@ -1791,7 +1785,7 @@
         <v>21</v>
       </c>
       <c r="C93">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D93">
         <v>24</v>
@@ -1816,10 +1810,10 @@
         <v>8931305</v>
       </c>
       <c r="B95">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C95">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D95">
         <v>25</v>
@@ -1841,7 +1835,7 @@
         <v>33</v>
       </c>
       <c r="C97">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D97">
         <v>25</v>
@@ -1852,10 +1846,10 @@
         <v>8976584</v>
       </c>
       <c r="B98">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C98">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D98">
         <v>27</v>
@@ -1866,10 +1860,10 @@
         <v>8985647</v>
       </c>
       <c r="B99">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C99">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D99">
         <v>18</v>
@@ -1897,10 +1891,10 @@
         <v>9020776</v>
       </c>
       <c r="B101">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C101">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D101">
         <v>27</v>
@@ -1914,7 +1908,7 @@
         <v>40</v>
       </c>
       <c r="C102">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D102">
         <v>24</v>
@@ -1925,10 +1919,10 @@
         <v>9049401</v>
       </c>
       <c r="B103">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C103">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D103">
         <v>22</v>
@@ -1953,10 +1947,10 @@
         <v>9086188</v>
       </c>
       <c r="B105">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C105">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D105">
         <v>20</v>
@@ -1975,10 +1969,10 @@
         <v>9115352</v>
       </c>
       <c r="B107">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C107">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D107">
         <v>20</v>
@@ -1989,10 +1983,10 @@
         <v>9118382</v>
       </c>
       <c r="B108">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C108">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D108">
         <v>21</v>

</xml_diff>

<commit_message>
Check in modified ground truth points
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_all.xlsx
+++ b/GHT/ground_truth_detection_pts_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\ESC499\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EF4EA2-DDD8-406B-BF3B-DD851C55A961}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9B3448-BD31-475C-9FCB-70339E1C00D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12098" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="G107" sqref="G107"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -676,7 +676,7 @@
         <v>19</v>
       </c>
       <c r="C14">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14">
         <v>19</v>
@@ -755,7 +755,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="2">
         <v>18</v>
@@ -895,10 +895,10 @@
         <v>6095054</v>
       </c>
       <c r="B29" s="2">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D29" s="2">
         <v>25</v>
@@ -920,10 +920,10 @@
         <v>6173842</v>
       </c>
       <c r="B31" s="2">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C31" s="2">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D31" s="2">
         <v>18</v>
@@ -934,10 +934,10 @@
         <v>6201211</v>
       </c>
       <c r="B32" s="2">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C32" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D32" s="2">
         <v>17</v>
@@ -954,7 +954,7 @@
         <v>26</v>
       </c>
       <c r="C33" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D33" s="2">
         <v>13</v>
@@ -1139,7 +1139,7 @@
         <v>31</v>
       </c>
       <c r="C46" s="2">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D46" s="2">
         <v>23</v>
@@ -1153,7 +1153,7 @@
         <v>30</v>
       </c>
       <c r="C47" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D47" s="2">
         <v>23</v>
@@ -1268,7 +1268,7 @@
         <v>27</v>
       </c>
       <c r="C55" s="2">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D55" s="2">
         <v>17</v>
@@ -1279,10 +1279,10 @@
         <v>7800424</v>
       </c>
       <c r="B56" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C56">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D56" s="2">
         <v>21</v>
@@ -1522,10 +1522,10 @@
         <v>8512802</v>
       </c>
       <c r="B74">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C74">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D74">
         <v>21</v>
@@ -1785,7 +1785,7 @@
         <v>21</v>
       </c>
       <c r="C93">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D93">
         <v>24</v>
@@ -1796,7 +1796,7 @@
         <v>8931170</v>
       </c>
       <c r="B94">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C94">
         <v>48</v>
@@ -1810,10 +1810,10 @@
         <v>8931305</v>
       </c>
       <c r="B95">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C95">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D95">
         <v>25</v>
@@ -2014,7 +2014,7 @@
         <v>20</v>
       </c>
       <c r="C110">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D110">
         <v>15</v>

</xml_diff>